<commit_message>
Changed Kenzi to red
</commit_message>
<xml_diff>
--- a/Assets/BandColorConvention/BandColorConvention.xlsx
+++ b/Assets/BandColorConvention/BandColorConvention.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Dev\TechnicalDocumentation\Assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\TechnicalDocumentation\Assets\BandColorConvention\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67D7839E-7813-4838-BBBB-A6E49DDFB8A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA64A28C-73F2-409C-B4FD-3C8D22348964}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{976BA9A3-41FE-45E5-BC0B-B40312D9AF21}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{976BA9A3-41FE-45E5-BC0B-B40312D9AF21}"/>
   </bookViews>
   <sheets>
     <sheet name="Document Style" sheetId="4" r:id="rId1"/>
@@ -86,9 +86,6 @@
     <t>Bass, Vocals</t>
   </si>
   <si>
-    <t>Magenta</t>
-  </si>
-  <si>
     <t>Position</t>
   </si>
   <si>
@@ -123,6 +120,9 @@
   </si>
   <si>
     <t>USC</t>
+  </si>
+  <si>
+    <t>Red</t>
   </si>
 </sst>
 </file>
@@ -184,7 +184,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF66FF"/>
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -222,8 +222,8 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -555,7 +555,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="385" zoomScaleNormal="385" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -575,29 +575,29 @@
         <v>6</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E2" s="6" t="s">
+      <c r="C2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>12</v>
       </c>
     </row>
@@ -609,10 +609,10 @@
         <v>1</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>24</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>25</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>15</v>
@@ -626,10 +626,10 @@
         <v>2</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>13</v>
@@ -643,29 +643,29 @@
         <v>3</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="5" t="s">
+      <c r="A6" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" s="5" t="s">
+      <c r="C6" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="D6" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="6" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Moved bass from John to Gordon
</commit_message>
<xml_diff>
--- a/Assets/BandColorConvention/BandColorConvention.xlsx
+++ b/Assets/BandColorConvention/BandColorConvention.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\TechnicalDocumentation\Assets\BandColorConvention\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Dev\TechnicalDocumentation\Assets\BandColorConvention\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A880F752-1DF4-42B6-8246-8F5A163DFBAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A8C00D2-87B0-4E22-97E9-3462EAB84E35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{976BA9A3-41FE-45E5-BC0B-B40312D9AF21}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{976BA9A3-41FE-45E5-BC0B-B40312D9AF21}"/>
   </bookViews>
   <sheets>
     <sheet name="Document Style" sheetId="4" r:id="rId1"/>
@@ -41,9 +41,6 @@
     <t>Chad</t>
   </si>
   <si>
-    <t>John</t>
-  </si>
-  <si>
     <t>Jessica</t>
   </si>
   <si>
@@ -123,6 +120,9 @@
   </si>
   <si>
     <t>Red</t>
+  </si>
+  <si>
+    <t>Gordon</t>
   </si>
 </sst>
 </file>
@@ -555,7 +555,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="385" zoomScaleNormal="385" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -569,104 +569,104 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>24</v>
-      </c>
       <c r="E3" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Excel files for Band Color Convention and Input List
</commit_message>
<xml_diff>
--- a/Assets/BandColorConvention/BandColorConvention.xlsx
+++ b/Assets/BandColorConvention/BandColorConvention.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Dev\TechnicalDocumentation\Assets\BandColorConvention\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\TechnicalDocumentation\Assets\BandColorConvention\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E41AE37A-B2AD-4A2E-85CC-6AF44B349D8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2448D76-61CE-4111-BD41-50CCF6C8CF17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="1305" windowWidth="29040" windowHeight="15720" xr2:uid="{976BA9A3-41FE-45E5-BC0B-B40312D9AF21}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{976BA9A3-41FE-45E5-BC0B-B40312D9AF21}"/>
   </bookViews>
   <sheets>
     <sheet name="Document Style" sheetId="4" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
   <si>
     <t>Chad</t>
   </si>
@@ -92,24 +92,9 @@
     <t>Upstage Center</t>
   </si>
   <si>
-    <t>DCR</t>
-  </si>
-  <si>
-    <t>DCL</t>
-  </si>
-  <si>
-    <t>Downstage Center Right</t>
-  </si>
-  <si>
-    <t>Downstage Center Left</t>
-  </si>
-  <si>
     <t>Downstage Right</t>
   </si>
   <si>
-    <t>DSR</t>
-  </si>
-  <si>
     <t>DSL</t>
   </si>
   <si>
@@ -123,6 +108,30 @@
   </si>
   <si>
     <t>Billy</t>
+  </si>
+  <si>
+    <t>Pink</t>
+  </si>
+  <si>
+    <t>???</t>
+  </si>
+  <si>
+    <t>Upstage Right</t>
+  </si>
+  <si>
+    <t>Downstage Center</t>
+  </si>
+  <si>
+    <t>Upstage Left</t>
+  </si>
+  <si>
+    <t>USR</t>
+  </si>
+  <si>
+    <t>DSC</t>
+  </si>
+  <si>
+    <t>USL</t>
   </si>
 </sst>
 </file>
@@ -152,7 +161,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -192,6 +201,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF00FF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -223,7 +238,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -231,6 +246,7 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -239,12 +255,12 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF00FF"/>
       <color rgb="FF0066FF"/>
       <color rgb="FF00E266"/>
       <color rgb="FFF2F2F2"/>
       <color rgb="FF99FF99"/>
       <color rgb="FFE2EFDA"/>
-      <color rgb="FFFF00FF"/>
       <color rgb="FF00B050"/>
       <color rgb="FF70AD47"/>
       <color rgb="FFFF66FF"/>
@@ -559,10 +575,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D0FC92A-968B-4411-B6B8-D166D6F99331}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -602,7 +618,7 @@
         <v>17</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>11</v>
@@ -613,13 +629,13 @@
         <v>9</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>14</v>
@@ -633,10 +649,10 @@
         <v>1</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>12</v>
@@ -650,7 +666,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>19</v>
@@ -661,19 +677,36 @@
     </row>
     <row r="6" spans="1:5" ht="33.75" x14ac:dyDescent="0.5">
       <c r="A6" s="6" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="33.75" x14ac:dyDescent="0.5">
+      <c r="A7" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>